<commit_message>
:bug: fix: tabela viagens
</commit_message>
<xml_diff>
--- a/EventosSazonais.xlsx
+++ b/EventosSazonais.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felps\Documents\Faculdade\1. Repositório Github\Algoritmo-Log\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felps\Documents\1.Falculdade\Repositórios GitHub\Algoritmo-Log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7E6D9AF-7FAB-46A0-8B67-EE150C568820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC0AE886-471D-477A-A395-7E8F398CBC50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8C9DEE2F-98E5-482A-A53C-84FBD4A207BA}"/>
+    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{8C9DEE2F-98E5-482A-A53C-84FBD4A207BA}"/>
   </bookViews>
   <sheets>
     <sheet name="eventosSazonais" sheetId="2" r:id="rId1"/>
@@ -507,17 +507,17 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -531,219 +531,219 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1">
-        <v>45332</v>
+        <v>44967</v>
       </c>
       <c r="C2" s="1">
-        <v>45336</v>
+        <v>44971</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1">
-        <v>45359</v>
+        <v>44993</v>
       </c>
       <c r="C3" s="1">
-        <v>45359</v>
+        <v>44993</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="1">
-        <v>45366</v>
+        <v>45000</v>
       </c>
       <c r="C4" s="1">
-        <v>45366</v>
+        <v>45000</v>
       </c>
       <c r="D4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="1">
-        <v>45399</v>
+        <v>45033</v>
       </c>
       <c r="C5" s="1">
-        <v>45399</v>
+        <v>45033</v>
       </c>
       <c r="D5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="1">
-        <v>45420</v>
+        <v>45054</v>
       </c>
       <c r="C6" s="1">
-        <v>45420</v>
+        <v>45054</v>
       </c>
       <c r="D6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="1">
-        <v>45455</v>
+        <v>45089</v>
       </c>
       <c r="C7" s="1">
-        <v>45455</v>
+        <v>45089</v>
       </c>
       <c r="D7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="1">
-        <v>45467</v>
+        <v>45101</v>
       </c>
       <c r="C8" s="1">
-        <v>45467</v>
+        <v>45101</v>
       </c>
       <c r="D8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="1">
-        <v>45471</v>
+        <v>45105</v>
       </c>
       <c r="C9" s="1">
-        <v>45471</v>
+        <v>45105</v>
       </c>
       <c r="D9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="1">
-        <v>45499</v>
+        <v>45133</v>
       </c>
       <c r="C10" s="1">
-        <v>45499</v>
+        <v>45133</v>
       </c>
       <c r="D10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="1">
-        <v>45515</v>
+        <v>45149</v>
       </c>
       <c r="C11" s="1">
-        <v>45515</v>
+        <v>45149</v>
       </c>
       <c r="D11" t="s">
         <v>19</v>
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="1">
-        <v>45577</v>
+        <v>45211</v>
       </c>
       <c r="C12" s="1">
-        <v>45577</v>
+        <v>45211</v>
       </c>
       <c r="D12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="1">
-        <v>45596</v>
+        <v>45230</v>
       </c>
       <c r="C13" s="1">
-        <v>45596</v>
+        <v>45230</v>
       </c>
       <c r="D13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="1">
-        <v>45625</v>
+        <v>45259</v>
       </c>
       <c r="C14" s="1">
-        <v>45625</v>
+        <v>45259</v>
       </c>
       <c r="D14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="1">
-        <v>45651</v>
+        <v>45285</v>
       </c>
       <c r="C15" s="1">
-        <v>45651</v>
+        <v>45285</v>
       </c>
       <c r="D15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
       <c r="B16" s="1">
-        <v>45658</v>
+        <v>44927</v>
       </c>
       <c r="C16" s="1">
-        <v>45658</v>
+        <v>44927</v>
       </c>
       <c r="D16" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>

</xml_diff>

<commit_message>
:bug: fix: Correção de bugs
</commit_message>
<xml_diff>
--- a/EventosSazonais.xlsx
+++ b/EventosSazonais.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felps\Documents\1.Falculdade\Repositórios GitHub\Algoritmo-Log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC0AE886-471D-477A-A395-7E8F398CBC50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E88DAA-D143-49FC-9831-68FB1D69CDBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{8C9DEE2F-98E5-482A-A53C-84FBD4A207BA}"/>
   </bookViews>
@@ -507,7 +507,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,10 +536,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="1">
-        <v>44967</v>
+        <v>44970</v>
       </c>
       <c r="C2" s="1">
-        <v>44971</v>
+        <v>44970</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>

</xml_diff>